<commit_message>
Agregados archivos csv a partir de la tabla de excel
</commit_message>
<xml_diff>
--- a/data/metadatos-bga.xlsx
+++ b/data/metadatos-bga.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Obra" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Referencias" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Referentes" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -53,46 +53,46 @@
     <t>el-paraiso.jpg</t>
   </si>
   <si>
+    <t>Zócalo de la tragedia</t>
+  </si>
+  <si>
+    <t>100x70</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tipografía sobre papel</t>
+  </si>
+  <si>
+    <t>zocalo-tragedia.jpg</t>
+  </si>
+  <si>
+    <t>Periodico</t>
+  </si>
+  <si>
+    <t>Doble suicidio en "El Sisga"</t>
+  </si>
+  <si>
+    <t>06-29-1965</t>
+  </si>
+  <si>
+    <t>El Tiempo</t>
+  </si>
+  <si>
+    <t>doble-suicidio-el-tiempo.jpg</t>
+  </si>
+  <si>
+    <t>Una indígena y su hijo murieron en persecución</t>
+  </si>
+  <si>
+    <t>05-24-1996</t>
+  </si>
+  <si>
+    <t>indigena-hijo-el-tiempo.jpg</t>
+  </si>
+  <si>
     <t>Láminas de paisajes latinoamericanos</t>
   </si>
   <si>
     <t>laminas-paisajes.jpg</t>
-  </si>
-  <si>
-    <t>Zócalo de la tragedia</t>
-  </si>
-  <si>
-    <t>100x70</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Tipografía sobre papel</t>
-  </si>
-  <si>
-    <t>zocalo-tragedia.jpg</t>
-  </si>
-  <si>
-    <t>Periodico</t>
-  </si>
-  <si>
-    <t>Doble suicidio en "El Sisga"</t>
-  </si>
-  <si>
-    <t>06-29-1965</t>
-  </si>
-  <si>
-    <t>El Tiempo</t>
-  </si>
-  <si>
-    <t>doble-suicidio-el-tiempo.jpg</t>
-  </si>
-  <si>
-    <t>Una indígena y su hijo murieron en persecución</t>
-  </si>
-  <si>
-    <t>05-24-1996</t>
-  </si>
-  <si>
-    <t>indigena-hijo-el-tiempo.jpg</t>
   </si>
   <si>
     <t>Exmilitar Mata a la Esposa de su Amigo y se Suicida</t>
@@ -453,34 +453,23 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1">
+      <c r="A4" s="5">
         <v>3.0</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="C4" s="6">
+        <v>30317.0</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="5">
-        <v>4.0</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="6">
-        <v>30317.0</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="F4" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -513,7 +502,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>5</v>
@@ -524,16 +513,16 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3">
@@ -541,21 +530,27 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5">
         <v>3.0</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5">

</xml_diff>